<commit_message>
Continued working on management. LB
</commit_message>
<xml_diff>
--- a/Plan ICT.xlsx
+++ b/Plan ICT.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
     <sheet name="Blatt2" sheetId="2" r:id="rId2"/>
+    <sheet name="Blatt3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>Auslöser</t>
   </si>
@@ -143,6 +144,63 @@
   </si>
   <si>
     <t>Blinken bei Frucht</t>
+  </si>
+  <si>
+    <t>Levelanstieg</t>
+  </si>
+  <si>
+    <t>GameOver</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>Spiel beenden</t>
+  </si>
+  <si>
+    <t>Weiterspielen</t>
+  </si>
+  <si>
+    <t>Zähler</t>
+  </si>
+  <si>
+    <t>Leben</t>
+  </si>
+  <si>
+    <t>Spielstand / Highscore</t>
+  </si>
+  <si>
+    <t>Desktop-Icon</t>
+  </si>
+  <si>
+    <t>Dokumentation</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Testkonzept</t>
+  </si>
+  <si>
+    <t>Hot-seat</t>
+  </si>
+  <si>
+    <t>Aurel / Lukas</t>
+  </si>
+  <si>
+    <t>Lukas</t>
+  </si>
+  <si>
+    <t>Pascal</t>
+  </si>
+  <si>
+    <t>Steuerung</t>
+  </si>
+  <si>
+    <t>Körner essen</t>
+  </si>
+  <si>
+    <t>Animation</t>
   </si>
 </sst>
 </file>
@@ -668,82 +726,187 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10">
+      <c r="I1">
+        <v>48</v>
+      </c>
+      <c r="J1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="B2" t="s">
+    <row r="3" spans="1:10">
+      <c r="B3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3" t="s">
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="C4" t="s">
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="C5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="D5" t="s">
+    <row r="6" spans="1:10">
+      <c r="D6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="D6" t="s">
+    <row r="7" spans="1:10">
+      <c r="D7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="C7" t="s">
+    <row r="8" spans="1:10">
+      <c r="C8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="C8" t="s">
+    <row r="9" spans="1:10">
+      <c r="C9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="B11" t="s">
+    <row r="12" spans="1:10">
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="C12" t="s">
+      <c r="G12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="C13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" t="s">
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="B14" t="s">
+    <row r="15" spans="1:10">
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="C15" t="s">
+    <row r="19" spans="1:3">
+      <c r="C19" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -755,4 +918,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>